<commit_message>
fix a big in the excel file (cost database)
</commit_message>
<xml_diff>
--- a/cost/Cost_Database.xlsx
+++ b/cost/Cost_Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannbn/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C8BC65-D624-6D44-9DBC-64945844CE1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2685A14C-B248-1A4E-AF35-E445ECBB630C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="17180" tabRatio="877" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="17180" tabRatio="877" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Database" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4620" uniqueCount="714">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4617" uniqueCount="714">
   <si>
     <t>Account</t>
   </si>
@@ -1911,9 +1911,6 @@
     <t>New Reactor Fueling Line Count</t>
   </si>
   <si>
-    <t xml:space="preserve">Reactor Testing Building </t>
-  </si>
-  <si>
     <t>Reactor Testing Hot Cell</t>
   </si>
   <si>
@@ -2251,6 +2248,9 @@
   </si>
   <si>
     <t>Annualized Helium Replenishment</t>
+  </si>
+  <si>
+    <t>Reactor Testing Building</t>
   </si>
 </sst>
 </file>
@@ -2266,7 +2266,7 @@
     <numFmt numFmtId="168" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="169" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;?_);_(@_)"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2388,12 +2388,6 @@
       <sz val="10"/>
       <color rgb="FF383A42"/>
       <name val="Menlo"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -2602,7 +2596,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2989,6 +2983,40 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="16" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3020,14 +3048,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3041,73 +3064,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3169,6 +3126,98 @@
       </font>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
       </font>
@@ -3197,109 +3246,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
@@ -3308,70 +3254,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3458,6 +3340,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
@@ -3465,7 +3361,45 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3519,9 +3453,84 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -3538,9 +3547,28 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3615,6 +3643,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
@@ -3630,6 +3665,34 @@
       <fill>
         <patternFill>
           <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3664,7 +3727,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3678,42 +3741,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3732,14 +3760,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3764,7 +3792,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3778,7 +3806,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3820,7 +3848,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3834,7 +3862,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3850,7 +3878,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3864,7 +3892,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3886,32 +3914,6 @@
       <fill>
         <patternFill>
           <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3949,7 +3951,33 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3963,7 +3991,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4005,13 +4033,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
@@ -4020,6 +4041,13 @@
       <fill>
         <patternFill>
           <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4084,7 +4112,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4098,7 +4126,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4110,7 +4138,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4124,7 +4152,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4149,16 +4177,155 @@
     <dxf>
       <font>
         <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
         <i/>
       </font>
       <fill>
         <patternFill patternType="gray0625"/>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -4196,59 +4363,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4269,6 +4384,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -4276,7 +4398,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4290,101 +4412,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4438,7 +4466,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4452,14 +4480,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4473,7 +4501,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4498,60 +4526,6 @@
       </font>
       <fill>
         <patternFill patternType="gray0625"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
       </fill>
     </dxf>
     <dxf>
@@ -4599,6 +4573,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
@@ -4607,6 +4588,53 @@
       <fill>
         <patternFill>
           <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFBA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4634,14 +4662,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4808,21 +4836,16 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
     </dxf>
     <dxf>
       <fill>
@@ -4856,6 +4879,11 @@
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -4912,7 +4940,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4926,14 +4954,9 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
     </dxf>
     <dxf>
       <fill>
@@ -4945,14 +4968,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4974,16 +4997,21 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
+          <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5005,14 +5033,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor rgb="FFFFFFBA"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFBA"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5340,7 +5368,7 @@
   <dimension ref="A1:AJ181"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="C173" sqref="C173"/>
     </sheetView>
@@ -19538,11 +19566,11 @@
     <cfRule type="expression" dxfId="298" priority="547">
       <formula>$B97=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="297" priority="548">
+    <cfRule type="expression" dxfId="297" priority="549">
+      <formula>$B97&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="296" priority="548">
       <formula>$B97=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="296" priority="549">
-      <formula>$B97&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A106:F108 U113:V119 U120:U121 A135:B140 N142:V142 N143:R143 U143:V148 K144:R144 A148:T148 T152:V157 A158:V161 A162:J163">
@@ -19561,17 +19589,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A150:R157">
-    <cfRule type="expression" dxfId="292" priority="656">
+    <cfRule type="expression" dxfId="292" priority="657">
+      <formula>$B150=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="291" priority="656">
       <formula>$B150=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="291" priority="657">
-      <formula>$B150=2</formula>
+    <cfRule type="expression" dxfId="290" priority="659">
+      <formula>$B150=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="290" priority="658">
+    <cfRule type="expression" dxfId="289" priority="658">
       <formula>$B150&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="289" priority="659">
-      <formula>$B150=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A124:S125 U124:V125 U166:V168">
@@ -19580,28 +19608,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105:U105">
-    <cfRule type="expression" dxfId="287" priority="764">
-      <formula>$B105=3</formula>
+    <cfRule type="expression" dxfId="287" priority="767">
+      <formula>$B105=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="286" priority="765">
       <formula>$B105=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="285" priority="766">
+    <cfRule type="expression" dxfId="285" priority="764">
+      <formula>$B105=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="284" priority="766">
       <formula>$B105&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="284" priority="767">
-      <formula>$B105=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A74:V96 A104:V104 A170:R176">
-    <cfRule type="expression" dxfId="283" priority="461">
-      <formula>$B74=3</formula>
+    <cfRule type="expression" dxfId="283" priority="463">
+      <formula>$B74&lt;2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="282" priority="462">
       <formula>$B74=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="281" priority="463">
-      <formula>$B74&lt;2</formula>
+    <cfRule type="expression" dxfId="281" priority="461">
+      <formula>$B74=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A76:V83">
@@ -19641,33 +19669,33 @@
     <cfRule type="expression" dxfId="273" priority="693">
       <formula>$B149=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="272" priority="694">
+    <cfRule type="expression" dxfId="272" priority="695">
+      <formula>$B149=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="271" priority="694">
       <formula>$B149&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="271" priority="695">
-      <formula>$B149=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A178:V181">
-    <cfRule type="expression" dxfId="270" priority="624">
+    <cfRule type="expression" dxfId="270" priority="627">
+      <formula>$B178=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="269" priority="624">
       <formula>$B178=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="269" priority="625">
+    <cfRule type="expression" dxfId="268" priority="625">
       <formula>$B178=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="268" priority="626">
+    <cfRule type="expression" dxfId="267" priority="626">
       <formula>$B178&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="267" priority="627">
-      <formula>$B178=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:AG4 A5:S6 U5:AG6 A106:F108 A109:V111 U113:V119 U120:U121 A124:S125 U124:V125 A135:B140 U135:V140 A141:V141 N142:V142 N143:R143 U143:V148 K144:R144 A148:T148 T152:V157 A158:V161 A162:J163 A164:L168 U166:V168">
-    <cfRule type="expression" dxfId="266" priority="761">
+    <cfRule type="expression" dxfId="266" priority="762">
+      <formula>$B1&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="265" priority="761">
       <formula>$B1=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="265" priority="762">
-      <formula>$B1&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:AG4 A5:S6 U5:AG6 A7:AG51 A170:R176">
@@ -19769,11 +19797,11 @@
     <cfRule type="expression" dxfId="241" priority="394">
       <formula>$B97=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="240" priority="395">
+    <cfRule type="expression" dxfId="240" priority="396">
+      <formula>$B97&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="239" priority="395">
       <formula>$B97=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="239" priority="396">
-      <formula>$B97&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99:C102">
@@ -19788,39 +19816,39 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101:C103">
-    <cfRule type="expression" dxfId="235" priority="380">
-      <formula>$B101=3</formula>
+    <cfRule type="expression" dxfId="235" priority="382">
+      <formula>$B101&lt;2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="234" priority="381">
       <formula>$B101=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="233" priority="382">
-      <formula>$B101&lt;2</formula>
+    <cfRule type="expression" dxfId="233" priority="380">
+      <formula>$B101=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C102:C103">
     <cfRule type="expression" dxfId="232" priority="26">
       <formula>$B102=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="231" priority="27">
+    <cfRule type="expression" dxfId="231" priority="28">
+      <formula>$B102&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="230" priority="27">
       <formula>$B102=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="230" priority="28">
-      <formula>$B102&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C135:T135 C136:R140">
-    <cfRule type="expression" dxfId="229" priority="583">
+    <cfRule type="expression" dxfId="229" priority="586">
+      <formula>$B135=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="228" priority="583">
       <formula>$B135=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="228" priority="584">
+    <cfRule type="expression" dxfId="227" priority="584">
       <formula>$B135=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="227" priority="585">
+    <cfRule type="expression" dxfId="226" priority="585">
       <formula>$B135&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="226" priority="586">
-      <formula>$B135=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D80 D82 D84:D134 D141:D181">
@@ -19864,25 +19892,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D97:E103">
-    <cfRule type="expression" dxfId="225" priority="373">
+    <cfRule type="expression" dxfId="225" priority="375">
+      <formula>$B97&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="224" priority="373">
       <formula>$B97=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="224" priority="374">
+    <cfRule type="expression" dxfId="223" priority="374">
       <formula>$B97=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="223" priority="375">
-      <formula>$B97&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E97:E103">
-    <cfRule type="expression" dxfId="222" priority="370">
+    <cfRule type="expression" dxfId="222" priority="372">
+      <formula>$B97&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="221" priority="370">
       <formula>$B97=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="221" priority="371">
+    <cfRule type="expression" dxfId="220" priority="371">
       <formula>$B97=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="220" priority="372">
-      <formula>$B97&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E83:Q83 Q124:Q125">
@@ -19901,25 +19929,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F111">
-    <cfRule type="expression" dxfId="216" priority="43">
-      <formula>$B111=3</formula>
+    <cfRule type="expression" dxfId="216" priority="45">
+      <formula>$B111&lt;2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="215" priority="44">
       <formula>$B111=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="214" priority="45">
-      <formula>$B111&lt;2</formula>
+    <cfRule type="expression" dxfId="214" priority="43">
+      <formula>$B111=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F109:G110">
-    <cfRule type="expression" dxfId="213" priority="46">
-      <formula>$B109=3</formula>
+    <cfRule type="expression" dxfId="213" priority="48">
+      <formula>$B109&lt;2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="212" priority="47">
       <formula>$B109=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="211" priority="48">
-      <formula>$B109&lt;2</formula>
+    <cfRule type="expression" dxfId="211" priority="46">
+      <formula>$B109=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F51:I54">
@@ -19948,36 +19976,36 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F97:I99 F100 H100:I100 F101:I101 F102 H102:I102">
-    <cfRule type="expression" dxfId="203" priority="162">
-      <formula>$B97=3</formula>
+    <cfRule type="expression" dxfId="203" priority="164">
+      <formula>$B97&lt;2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="202" priority="163">
       <formula>$B97=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="201" priority="164">
-      <formula>$B97&lt;2</formula>
+    <cfRule type="expression" dxfId="201" priority="162">
+      <formula>$B97=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F99:I101">
     <cfRule type="expression" dxfId="200" priority="32">
       <formula>$B99=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="199" priority="33">
+    <cfRule type="expression" dxfId="199" priority="34">
+      <formula>$B99&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="198" priority="33">
       <formula>$B99=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="198" priority="34">
-      <formula>$B99&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F102:I103">
-    <cfRule type="expression" dxfId="197" priority="7">
-      <formula>$B102=3</formula>
+    <cfRule type="expression" dxfId="197" priority="9">
+      <formula>$B102&lt;2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="196" priority="8">
       <formula>$B102=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="195" priority="9">
-      <formula>$B102&lt;2</formula>
+    <cfRule type="expression" dxfId="195" priority="7">
+      <formula>$B102=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F103:I103">
@@ -20002,36 +20030,36 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G100">
-    <cfRule type="expression" dxfId="189" priority="29">
-      <formula>$B100=3</formula>
+    <cfRule type="expression" dxfId="189" priority="31">
+      <formula>$B100&lt;2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="188" priority="30">
       <formula>$B100=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="187" priority="31">
-      <formula>$B100&lt;2</formula>
+    <cfRule type="expression" dxfId="187" priority="29">
+      <formula>$B100=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G102">
-    <cfRule type="expression" dxfId="186" priority="4">
-      <formula>$B102=3</formula>
+    <cfRule type="expression" dxfId="186" priority="6">
+      <formula>$B102&lt;2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="185" priority="5">
       <formula>$B102=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="184" priority="6">
-      <formula>$B102&lt;2</formula>
+    <cfRule type="expression" dxfId="184" priority="4">
+      <formula>$B102=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G106:I107">
-    <cfRule type="expression" dxfId="183" priority="756">
-      <formula>$B106=3</formula>
+    <cfRule type="expression" dxfId="183" priority="758">
+      <formula>$B106&lt;2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="182" priority="757">
       <formula>$B106=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="181" priority="758">
-      <formula>$B106&lt;2</formula>
+    <cfRule type="expression" dxfId="181" priority="756">
+      <formula>$B106=3</formula>
     </cfRule>
     <cfRule type="expression" dxfId="180" priority="759">
       <formula>$B106=0</formula>
@@ -20049,36 +20077,36 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H145:H146">
-    <cfRule type="expression" dxfId="176" priority="1031">
-      <formula>$B146=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="175" priority="1032">
+    <cfRule type="expression" dxfId="176" priority="1032">
       <formula>$B146&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="174" priority="1034">
+    <cfRule type="expression" dxfId="175" priority="1034">
       <formula>$B146=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="174" priority="1031">
+      <formula>$B146=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5">
-    <cfRule type="expression" dxfId="173" priority="562">
-      <formula>$B5=3</formula>
+    <cfRule type="expression" dxfId="173" priority="563">
+      <formula>$B5=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="172" priority="563">
-      <formula>$B5=2</formula>
+    <cfRule type="expression" dxfId="172" priority="565">
+      <formula>$B5=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="171" priority="564">
       <formula>$B5&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="170" priority="565">
-      <formula>$B5=0</formula>
+    <cfRule type="expression" dxfId="170" priority="562">
+      <formula>$B5=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J71:L73">
-    <cfRule type="expression" dxfId="169" priority="613">
+    <cfRule type="expression" dxfId="169" priority="617">
+      <formula>$B71=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="168" priority="613">
       <formula>_xlfn.ISFORMULA(J71)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="168" priority="617">
-      <formula>$B71=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:Q96 J104:Q1048576">
@@ -20092,14 +20120,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J69:S73">
-    <cfRule type="expression" dxfId="165" priority="609">
-      <formula>$B69=3</formula>
+    <cfRule type="expression" dxfId="165" priority="611">
+      <formula>$B69&lt;2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="164" priority="610">
       <formula>$B69=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="163" priority="611">
-      <formula>$B69&lt;2</formula>
+    <cfRule type="expression" dxfId="163" priority="609">
+      <formula>$B69=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J68:V68 J69:S70 U69:V73">
@@ -20108,14 +20136,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J68:V68 U69:V73">
-    <cfRule type="expression" dxfId="161" priority="619">
-      <formula>$B68=3</formula>
+    <cfRule type="expression" dxfId="161" priority="621">
+      <formula>$B68&lt;2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="160" priority="620">
       <formula>$B68=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="159" priority="621">
-      <formula>$B68&lt;2</formula>
+    <cfRule type="expression" dxfId="159" priority="619">
+      <formula>$B68=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K81">
@@ -20151,14 +20179,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K97:M101">
-    <cfRule type="expression" dxfId="150" priority="132">
+    <cfRule type="expression" dxfId="150" priority="134">
+      <formula>$B97&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="149" priority="132">
       <formula>$B97=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="149" priority="133">
+    <cfRule type="expression" dxfId="148" priority="133">
       <formula>$B97=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="148" priority="134">
-      <formula>$B97&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K97:M103">
@@ -20181,33 +20209,33 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K102:M102">
-    <cfRule type="expression" dxfId="142" priority="23">
-      <formula>$B102=3</formula>
+    <cfRule type="expression" dxfId="142" priority="25">
+      <formula>$B102&lt;2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="141" priority="24">
       <formula>$B102=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="140" priority="25">
-      <formula>$B102&lt;2</formula>
+    <cfRule type="expression" dxfId="140" priority="23">
+      <formula>$B102=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K142:M143">
     <cfRule type="expression" dxfId="139" priority="720">
       <formula>$B142=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="138" priority="721">
-      <formula>$B142=2</formula>
+    <cfRule type="expression" dxfId="138" priority="723">
+      <formula>$B142=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="137" priority="722">
       <formula>$B142&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="136" priority="723">
-      <formula>$B142=0</formula>
+    <cfRule type="expression" dxfId="136" priority="721">
+      <formula>$B142=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L112">
-    <cfRule type="expression" dxfId="135" priority="569">
-      <formula>$B112=0</formula>
+    <cfRule type="expression" dxfId="135" priority="962">
+      <formula>#REF!=3</formula>
     </cfRule>
     <cfRule type="expression" dxfId="134" priority="959">
       <formula>#REF!=2</formula>
@@ -20215,11 +20243,11 @@
     <cfRule type="expression" dxfId="133" priority="960">
       <formula>#REF!&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="132" priority="961">
+    <cfRule type="expression" dxfId="132" priority="569">
+      <formula>$B112=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="131" priority="961">
       <formula>#REF!=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="131" priority="962">
-      <formula>#REF!=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L112:V112">
@@ -20234,14 +20262,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M103">
-    <cfRule type="expression" dxfId="127" priority="170">
-      <formula>$B103=3</formula>
+    <cfRule type="expression" dxfId="127" priority="172">
+      <formula>$B103&lt;2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="126" priority="171">
       <formula>$B103=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="172">
-      <formula>$B103&lt;2</formula>
+    <cfRule type="expression" dxfId="125" priority="170">
+      <formula>$B103=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N81">
@@ -20250,14 +20278,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O97:O98">
-    <cfRule type="expression" dxfId="123" priority="290">
-      <formula>$B97=3</formula>
+    <cfRule type="expression" dxfId="123" priority="292">
+      <formula>$B97&lt;2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="122" priority="291">
       <formula>$B97=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="121" priority="292">
-      <formula>$B97&lt;2</formula>
+    <cfRule type="expression" dxfId="121" priority="290">
+      <formula>$B97=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O97:O103">
@@ -20278,14 +20306,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O99:O103">
-    <cfRule type="expression" dxfId="115" priority="278">
-      <formula>$B99=3</formula>
+    <cfRule type="expression" dxfId="115" priority="280">
+      <formula>$B99&lt;2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="114" priority="279">
       <formula>$B99=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="280">
-      <formula>$B99&lt;2</formula>
+    <cfRule type="expression" dxfId="113" priority="278">
+      <formula>$B99=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q71:Q73">
@@ -20299,11 +20327,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q149">
-    <cfRule type="expression" dxfId="110" priority="777">
+    <cfRule type="expression" dxfId="110" priority="778">
+      <formula>$B150=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="109" priority="777">
       <formula>$B150=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="109" priority="778">
-      <formula>$B150=2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="108" priority="779">
       <formula>$B150&lt;2</formula>
@@ -20313,58 +20341,58 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q97:R98">
-    <cfRule type="expression" dxfId="106" priority="258">
+    <cfRule type="expression" dxfId="106" priority="259">
+      <formula>$B97=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="105" priority="258">
       <formula>$B97=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="105" priority="259">
-      <formula>$B97=2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="104" priority="260">
       <formula>$B97&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q97:R100">
-    <cfRule type="expression" dxfId="103" priority="251">
+    <cfRule type="expression" dxfId="103" priority="253">
+      <formula>$B97&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="102" priority="251">
       <formula>$B97=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="252">
+    <cfRule type="expression" dxfId="101" priority="252">
       <formula>$B97=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="101" priority="253">
-      <formula>$B97&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q101:R101">
-    <cfRule type="expression" dxfId="100" priority="100">
-      <formula>$B101=3</formula>
+    <cfRule type="expression" dxfId="100" priority="102">
+      <formula>$B101&lt;2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="99" priority="101">
       <formula>$B101=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="102">
-      <formula>$B101&lt;2</formula>
+    <cfRule type="expression" dxfId="98" priority="100">
+      <formula>$B101=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q102:R102">
-    <cfRule type="expression" dxfId="97" priority="20">
-      <formula>$B102=3</formula>
+    <cfRule type="expression" dxfId="97" priority="22">
+      <formula>$B102&lt;2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="96" priority="21">
       <formula>$B102=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="22">
-      <formula>$B102&lt;2</formula>
+    <cfRule type="expression" dxfId="95" priority="20">
+      <formula>$B102=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q103:R103">
-    <cfRule type="expression" dxfId="94" priority="93">
-      <formula>$B103=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="93" priority="94">
+    <cfRule type="expression" dxfId="94" priority="94">
       <formula>$B103=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="95">
+    <cfRule type="expression" dxfId="93" priority="95">
       <formula>$B103&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="92" priority="93">
+      <formula>$B103=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q71:S73">
@@ -20406,14 +20434,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q103:S103">
-    <cfRule type="expression" dxfId="81" priority="86">
-      <formula>$B103=3</formula>
+    <cfRule type="expression" dxfId="81" priority="88">
+      <formula>$B103&lt;2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="80" priority="87">
       <formula>$B103=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="88">
-      <formula>$B103&lt;2</formula>
+    <cfRule type="expression" dxfId="79" priority="86">
+      <formula>$B103=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q97:T103">
@@ -20422,53 +20450,53 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S97:S100">
-    <cfRule type="expression" dxfId="77" priority="237">
-      <formula>$B97=3</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="76" priority="238">
+    <cfRule type="expression" dxfId="77" priority="238">
       <formula>$B97=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="239">
+    <cfRule type="expression" dxfId="76" priority="239">
       <formula>$B97&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="75" priority="237">
+      <formula>$B97=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S102">
     <cfRule type="expression" dxfId="74" priority="14">
       <formula>$B102=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="15">
+    <cfRule type="expression" dxfId="73" priority="16">
+      <formula>$B102&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="72" priority="15">
       <formula>$B102=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="72" priority="16">
-      <formula>$B102&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S152">
-    <cfRule type="expression" dxfId="71" priority="704">
-      <formula>$B152=3</formula>
+    <cfRule type="expression" dxfId="71" priority="707">
+      <formula>$B152=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="70" priority="705">
       <formula>$B152=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="706">
+    <cfRule type="expression" dxfId="69" priority="704">
+      <formula>$B152=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="68" priority="706">
       <formula>$B152&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="68" priority="707">
-      <formula>$B152=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S156:S157">
     <cfRule type="expression" dxfId="67" priority="700">
       <formula>$B156=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="701">
-      <formula>$B156=2</formula>
+    <cfRule type="expression" dxfId="66" priority="703">
+      <formula>$B156=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="65" priority="702">
       <formula>$B156&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="703">
-      <formula>$B156=0</formula>
+    <cfRule type="expression" dxfId="64" priority="701">
+      <formula>$B156=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S97:T98">
@@ -20497,11 +20525,11 @@
     <cfRule type="expression" dxfId="57" priority="65">
       <formula>$B103=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="66">
+    <cfRule type="expression" dxfId="56" priority="67">
+      <formula>$B103&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="55" priority="66">
       <formula>$B103=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="55" priority="67">
-      <formula>$B103&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S90:V93">
@@ -20510,45 +20538,45 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S150:V151">
-    <cfRule type="expression" dxfId="53" priority="664">
-      <formula>$B150=3</formula>
+    <cfRule type="expression" dxfId="53" priority="667">
+      <formula>$B150=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="52" priority="665">
       <formula>$B150=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="666">
+    <cfRule type="expression" dxfId="51" priority="664">
+      <formula>$B150=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="50" priority="666">
       <formula>$B150&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="50" priority="667">
-      <formula>$B150=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5">
-    <cfRule type="expression" dxfId="49" priority="457">
-      <formula>$B5=0</formula>
+    <cfRule type="expression" dxfId="49" priority="460">
+      <formula>$B5&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="458">
+    <cfRule type="expression" dxfId="48" priority="459">
+      <formula>$B5=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="47" priority="458">
       <formula>$B5=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="459">
-      <formula>$B5=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="46" priority="460">
-      <formula>$B5&lt;2</formula>
+    <cfRule type="expression" dxfId="46" priority="457">
+      <formula>$B5=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T6">
-    <cfRule type="expression" dxfId="45" priority="1015">
+    <cfRule type="expression" dxfId="45" priority="1020">
+      <formula>$B5=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="1015">
       <formula>$B5=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="1016">
+    <cfRule type="expression" dxfId="43" priority="1016">
       <formula>$B5&lt;2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="1018">
+    <cfRule type="expression" dxfId="42" priority="1018">
       <formula>$B5=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="42" priority="1020">
-      <formula>$B5=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T97:T100">
@@ -20577,11 +20605,11 @@
     <cfRule type="expression" dxfId="35" priority="1">
       <formula>$B100=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="2">
+    <cfRule type="expression" dxfId="34" priority="3">
+      <formula>$B100&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="2">
       <formula>$B100=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="33" priority="3">
-      <formula>$B100&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T102:T103">
@@ -20596,17 +20624,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U106">
-    <cfRule type="expression" dxfId="29" priority="785">
-      <formula>$B105=3</formula>
+    <cfRule type="expression" dxfId="29" priority="788">
+      <formula>$B105=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="786">
+    <cfRule type="expression" dxfId="28" priority="787">
+      <formula>$B105&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="786">
       <formula>$B105=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="787">
-      <formula>$B105&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="788">
-      <formula>$B105=0</formula>
+    <cfRule type="expression" dxfId="26" priority="785">
+      <formula>$B105=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U135:AG140">
@@ -20615,39 +20643,39 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W97:W103">
-    <cfRule type="expression" dxfId="24" priority="212">
+    <cfRule type="expression" dxfId="24" priority="214">
+      <formula>$B97&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="212">
       <formula>$B97=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="213">
+    <cfRule type="expression" dxfId="22" priority="213">
       <formula>$B97=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="214">
-      <formula>$B97&lt;2</formula>
     </cfRule>
     <cfRule type="expression" dxfId="21" priority="215">
       <formula>$B97=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W76:AG82">
-    <cfRule type="expression" dxfId="20" priority="505">
-      <formula>$B76=3</formula>
+    <cfRule type="expression" dxfId="20" priority="508">
+      <formula>$B76=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="506">
+    <cfRule type="expression" dxfId="19" priority="507">
+      <formula>$B76&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="506">
       <formula>$B76=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="507">
-      <formula>$B76&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="508">
-      <formula>$B76=0</formula>
+    <cfRule type="expression" dxfId="17" priority="505">
+      <formula>$B76=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W95:AG96 A145:G146 I145:R146 A147:R147">
-    <cfRule type="expression" dxfId="16" priority="709">
+    <cfRule type="expression" dxfId="16" priority="710">
+      <formula>$B95&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="709">
       <formula>$B95=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="15" priority="710">
-      <formula>$B95&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W106:AG108">
@@ -20681,17 +20709,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z97:AG103">
-    <cfRule type="expression" dxfId="6" priority="54">
-      <formula>$B97=3</formula>
+    <cfRule type="expression" dxfId="6" priority="57">
+      <formula>$B97=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="55">
+    <cfRule type="expression" dxfId="5" priority="56">
+      <formula>$B97&lt;2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="55">
       <formula>$B97=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="56">
-      <formula>$B97&lt;2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="57">
-      <formula>$B97=0</formula>
+    <cfRule type="expression" dxfId="3" priority="54">
+      <formula>$B97=3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z133:AG133">
@@ -22377,7 +22405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="117" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -23698,8 +23726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AG268"/>
   <sheetViews>
-    <sheetView topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="C155" sqref="C155"/>
+    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="110" workbookViewId="0">
+      <selection activeCell="D131" sqref="D131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -23711,6 +23739,7 @@
     <col min="5" max="5" width="13.33203125" customWidth="1"/>
     <col min="6" max="8" width="13.6640625" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" customWidth="1"/>
     <col min="12" max="12" width="10" customWidth="1"/>
     <col min="13" max="13" width="15.6640625" customWidth="1"/>
     <col min="14" max="14" width="8.6640625" customWidth="1"/>
@@ -23724,8 +23753,10 @@
     <col min="22" max="22" width="116.83203125" customWidth="1"/>
     <col min="23" max="23" width="21.5" customWidth="1"/>
     <col min="24" max="24" width="16.6640625" customWidth="1"/>
-    <col min="26" max="26" width="12.5" customWidth="1"/>
+    <col min="25" max="25" width="13.5" customWidth="1"/>
+    <col min="26" max="26" width="16.1640625" customWidth="1"/>
     <col min="27" max="27" width="16.6640625" customWidth="1"/>
+    <col min="28" max="28" width="11" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="12.5" customWidth="1"/>
     <col min="30" max="30" width="6.6640625" customWidth="1"/>
     <col min="33" max="33" width="16.1640625" customWidth="1"/>
@@ -30573,11 +30604,11 @@
         <v>3</v>
       </c>
       <c r="C85" s="102" t="s">
-        <v>600</v>
+        <v>713</v>
       </c>
       <c r="D85" s="97" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">                  Reactor Testing Building </v>
+        <f>REPT("   ", B85*2) &amp; C85</f>
+        <v xml:space="preserve">                  Reactor Testing Building</v>
       </c>
       <c r="E85" s="97"/>
       <c r="F85" s="97"/>
@@ -30619,11 +30650,11 @@
       </c>
       <c r="C86" s="102" t="str">
         <f>_xlfn.CONCAT(C85," Roof")</f>
-        <v>Reactor Testing Building  Roof</v>
+        <v>Reactor Testing Building Roof</v>
       </c>
       <c r="D86" s="97" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                        Reactor Testing Building  Roof</v>
+        <v xml:space="preserve">                        Reactor Testing Building Roof</v>
       </c>
       <c r="E86" s="97" t="s">
         <v>35</v>
@@ -30646,7 +30677,7 @@
       </c>
       <c r="M86" s="102" t="str">
         <f>_xlfn.CONCAT(C86, " Volume")</f>
-        <v>Reactor Testing Building  Roof Volume</v>
+        <v>Reactor Testing Building Roof Volume</v>
       </c>
       <c r="N86" s="105"/>
       <c r="O86" s="104" t="s">
@@ -30717,11 +30748,11 @@
       </c>
       <c r="C87" s="102" t="str">
         <f>_xlfn.CONCAT(C85," Basement")</f>
-        <v>Reactor Testing Building  Basement</v>
+        <v>Reactor Testing Building Basement</v>
       </c>
       <c r="D87" s="97" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                        Reactor Testing Building  Basement</v>
+        <v xml:space="preserve">                        Reactor Testing Building Basement</v>
       </c>
       <c r="E87" s="97" t="s">
         <v>35</v>
@@ -30744,7 +30775,7 @@
       </c>
       <c r="M87" s="102" t="str">
         <f>_xlfn.CONCAT(C87, " Volume")</f>
-        <v>Reactor Testing Building  Basement Volume</v>
+        <v>Reactor Testing Building Basement Volume</v>
       </c>
       <c r="N87" s="105"/>
       <c r="O87" s="104" t="s">
@@ -30809,11 +30840,11 @@
       </c>
       <c r="C88" s="102" t="str">
         <f>_xlfn.CONCAT(C85," Walls")</f>
-        <v>Reactor Testing Building  Walls</v>
+        <v>Reactor Testing Building Walls</v>
       </c>
       <c r="D88" s="97" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                        Reactor Testing Building  Walls</v>
+        <v xml:space="preserve">                        Reactor Testing Building Walls</v>
       </c>
       <c r="E88" s="97" t="s">
         <v>35</v>
@@ -30836,7 +30867,7 @@
       </c>
       <c r="M88" s="102" t="str">
         <f>_xlfn.CONCAT(C88, " Volume")</f>
-        <v>Reactor Testing Building  Walls Volume</v>
+        <v>Reactor Testing Building Walls Volume</v>
       </c>
       <c r="N88" s="105"/>
       <c r="O88" s="104" t="s">
@@ -30900,7 +30931,7 @@
         <v>4</v>
       </c>
       <c r="C89" s="102" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D89" s="97" t="str">
         <f t="shared" si="3"/>
@@ -30910,7 +30941,7 @@
         <v>35</v>
       </c>
       <c r="F89" s="97" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G89" s="98"/>
       <c r="H89" s="97"/>
@@ -31074,7 +31105,7 @@
       <c r="L91" s="105"/>
       <c r="M91" s="102" t="str">
         <f>_xlfn.CONCAT(C85, " Volume")</f>
-        <v>Reactor Testing Building  Volume</v>
+        <v>Reactor Testing Building Volume</v>
       </c>
       <c r="N91" s="105"/>
       <c r="O91" s="105"/>
@@ -31132,7 +31163,7 @@
         <v>3</v>
       </c>
       <c r="C92" s="102" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D92" s="97" t="str">
         <f t="shared" si="3"/>
@@ -31543,7 +31574,7 @@
         <v>3</v>
       </c>
       <c r="C97" s="102" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D97" s="97" t="str">
         <f t="shared" si="3"/>
@@ -31980,7 +32011,7 @@
         <v>571</v>
       </c>
       <c r="M102" s="104" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="N102" s="105"/>
       <c r="O102" s="104"/>
@@ -32055,7 +32086,7 @@
         <v>2</v>
       </c>
       <c r="C103" s="102" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D103" s="97" t="str">
         <f t="shared" si="3"/>
@@ -32107,7 +32138,7 @@
         <v>3</v>
       </c>
       <c r="C104" s="102" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D104" s="97" t="str">
         <f t="shared" si="3"/>
@@ -32448,7 +32479,7 @@
         <v>4</v>
       </c>
       <c r="C108" s="102" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D108" s="97" t="str">
         <f t="shared" si="3"/>
@@ -32625,7 +32656,7 @@
         <v>80</v>
       </c>
       <c r="M110" s="102" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="N110" s="105"/>
       <c r="O110" s="104" t="s">
@@ -32685,7 +32716,7 @@
         <v>3</v>
       </c>
       <c r="C111" s="102" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D111" s="97" t="str">
         <f t="shared" si="3"/>
@@ -33035,7 +33066,7 @@
         <v>80</v>
       </c>
       <c r="M115" s="102" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="N115" s="105"/>
       <c r="O115" s="104" t="s">
@@ -33102,7 +33133,7 @@
         <v>3</v>
       </c>
       <c r="C116" s="102" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D116" s="97" t="str">
         <f t="shared" ref="D116:D179" si="7">REPT("   ", B116*2) &amp; C116</f>
@@ -33548,7 +33579,7 @@
         <v>3</v>
       </c>
       <c r="C121" s="102" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="D121" s="97" t="str">
         <f t="shared" si="7"/>
@@ -33959,7 +33990,7 @@
         <v>3</v>
       </c>
       <c r="C126" s="102" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D126" s="97" t="str">
         <f t="shared" si="7"/>
@@ -34396,7 +34427,7 @@
         <v>571</v>
       </c>
       <c r="M131" s="102" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="N131" s="105"/>
       <c r="O131" s="104"/>
@@ -34455,96 +34486,96 @@
         <v>48</v>
       </c>
     </row>
-    <row r="132" spans="1:33" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="94">
+    <row r="132" spans="1:33" s="165" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="152">
         <v>22</v>
       </c>
-      <c r="B132" s="96">
+      <c r="B132" s="153">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="C132" s="118" t="s">
-        <v>616</v>
-      </c>
-      <c r="D132" s="97" t="str">
+      <c r="C132" s="154" t="s">
+        <v>615</v>
+      </c>
+      <c r="D132" s="155" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve">      Manufacturing Facility Equipment</v>
       </c>
-      <c r="E132" s="97" t="s">
+      <c r="E132" s="155" t="s">
         <v>35</v>
       </c>
-      <c r="F132" s="97" t="s">
+      <c r="F132" s="155" t="s">
+        <v>616</v>
+      </c>
+      <c r="G132" s="156">
+        <v>1</v>
+      </c>
+      <c r="H132" s="155"/>
+      <c r="I132" s="155"/>
+      <c r="J132" s="157"/>
+      <c r="K132" s="157">
+        <v>74748072.817566499</v>
+      </c>
+      <c r="L132" s="158" t="s">
         <v>617</v>
       </c>
-      <c r="G132" s="98">
+      <c r="M132" s="155" t="s">
+        <v>616</v>
+      </c>
+      <c r="N132" s="159">
         <v>1</v>
       </c>
-      <c r="H132" s="97"/>
-      <c r="I132" s="97"/>
-      <c r="J132" s="103"/>
-      <c r="K132" s="103">
-        <v>74748072.817566499</v>
-      </c>
-      <c r="L132" s="105" t="s">
+      <c r="O132" s="159" t="s">
+        <v>617</v>
+      </c>
+      <c r="P132" s="160">
+        <v>-0.97870000000000001</v>
+      </c>
+      <c r="Q132" s="160">
+        <v>2024</v>
+      </c>
+      <c r="R132" s="159" t="s">
+        <v>86</v>
+      </c>
+      <c r="S132" s="161" t="s">
         <v>618</v>
       </c>
-      <c r="M132" s="97" t="s">
-        <v>617</v>
-      </c>
-      <c r="N132" s="109">
-        <v>1</v>
-      </c>
-      <c r="O132" s="109" t="s">
-        <v>618</v>
-      </c>
-      <c r="P132" s="106">
-        <v>-0.97870000000000001</v>
-      </c>
-      <c r="Q132" s="106">
-        <v>2024</v>
-      </c>
-      <c r="R132" s="109" t="s">
-        <v>86</v>
-      </c>
-      <c r="S132" s="119" t="s">
-        <v>619</v>
-      </c>
-      <c r="T132" s="109"/>
-      <c r="U132" s="109"/>
-      <c r="V132" s="109"/>
-      <c r="W132" s="100"/>
-      <c r="X132" s="110">
+      <c r="T132" s="159"/>
+      <c r="U132" s="159"/>
+      <c r="V132" s="159"/>
+      <c r="W132" s="162"/>
+      <c r="X132" s="163">
         <f>0.8*$I132</f>
         <v>0</v>
       </c>
-      <c r="Y132" s="110">
+      <c r="Y132" s="163">
         <f>2*J132</f>
         <v>0</v>
       </c>
-      <c r="Z132" s="100" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA132" s="101">
+      <c r="Z132" s="162" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA132" s="164">
         <f>0.8*K132</f>
         <v>59798458.254053205</v>
       </c>
-      <c r="AB132" s="101">
+      <c r="AB132" s="164">
         <f>2*K132</f>
         <v>149496145.635133</v>
       </c>
-      <c r="AC132" s="100" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD132" s="101" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE132" s="101" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF132" s="101" t="s">
-        <v>47</v>
-      </c>
-      <c r="AG132" s="100" t="s">
+      <c r="AC132" s="162" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD132" s="164">
+        <v>0.1</v>
+      </c>
+      <c r="AE132" s="164">
+        <v>0</v>
+      </c>
+      <c r="AF132" s="164">
+        <v>-1</v>
+      </c>
+      <c r="AG132" s="162" t="s">
         <v>48</v>
       </c>
     </row>
@@ -34557,7 +34588,7 @@
         <v>1</v>
       </c>
       <c r="C133" s="118" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D133" s="97" t="str">
         <f t="shared" si="7"/>
@@ -34602,7 +34633,7 @@
         <v>2</v>
       </c>
       <c r="C134" s="118" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D134" s="97" t="str">
         <f t="shared" si="7"/>
@@ -34647,7 +34678,7 @@
         <v>3</v>
       </c>
       <c r="C135" s="118" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D135" s="97" t="str">
         <f t="shared" si="7"/>
@@ -34657,7 +34688,7 @@
         <v>35</v>
       </c>
       <c r="F135" s="97" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G135" s="98">
         <v>12</v>
@@ -34680,12 +34711,12 @@
         <v>86</v>
       </c>
       <c r="S135" s="119" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="T135" s="109"/>
       <c r="U135" s="109"/>
       <c r="V135" s="109" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="W135" s="100" t="s">
         <v>43</v>
@@ -34732,7 +34763,7 @@
         <v>3</v>
       </c>
       <c r="C136" s="118" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D136" s="97" t="str">
         <f t="shared" si="7"/>
@@ -34742,7 +34773,7 @@
         <v>35</v>
       </c>
       <c r="F136" s="97" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G136" s="98">
         <v>2</v>
@@ -34765,12 +34796,12 @@
         <v>86</v>
       </c>
       <c r="S136" s="119" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="T136" s="109"/>
       <c r="U136" s="109"/>
       <c r="V136" s="109" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="W136" s="100" t="s">
         <v>43</v>
@@ -34817,7 +34848,7 @@
         <v>3</v>
       </c>
       <c r="C137" s="118" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D137" s="97" t="str">
         <f t="shared" si="7"/>
@@ -34827,7 +34858,7 @@
         <v>35</v>
       </c>
       <c r="F137" s="97" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G137" s="98">
         <v>1</v>
@@ -34850,12 +34881,12 @@
         <v>86</v>
       </c>
       <c r="S137" s="119" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="T137" s="109"/>
       <c r="U137" s="109"/>
       <c r="V137" s="109" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="W137" s="100" t="s">
         <v>43</v>
@@ -34902,7 +34933,7 @@
         <v>3</v>
       </c>
       <c r="C138" s="118" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D138" s="97" t="str">
         <f t="shared" si="7"/>
@@ -34912,7 +34943,7 @@
         <v>35</v>
       </c>
       <c r="F138" s="97" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G138" s="98">
         <v>2</v>
@@ -34979,7 +35010,7 @@
         <v>3</v>
       </c>
       <c r="C139" s="118" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D139" s="97" t="str">
         <f t="shared" si="7"/>
@@ -34989,7 +35020,7 @@
         <v>35</v>
       </c>
       <c r="F139" s="97" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G139" s="98">
         <v>1</v>
@@ -35012,16 +35043,16 @@
         <v>86</v>
       </c>
       <c r="S139" s="119" t="s">
+        <v>630</v>
+      </c>
+      <c r="T139" s="119" t="s">
         <v>631</v>
       </c>
-      <c r="T139" s="119" t="s">
+      <c r="U139" s="120" t="s">
         <v>632</v>
       </c>
-      <c r="U139" s="120" t="s">
+      <c r="V139" s="109" t="s">
         <v>633</v>
-      </c>
-      <c r="V139" s="109" t="s">
-        <v>634</v>
       </c>
       <c r="W139" s="100" t="s">
         <v>43</v>
@@ -35068,7 +35099,7 @@
         <v>3</v>
       </c>
       <c r="C140" s="118" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D140" s="97" t="str">
         <f t="shared" si="7"/>
@@ -35078,7 +35109,7 @@
         <v>35</v>
       </c>
       <c r="F140" s="97" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G140" s="98">
         <v>1</v>
@@ -35145,7 +35176,7 @@
         <v>3</v>
       </c>
       <c r="C141" s="118" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D141" s="97" t="str">
         <f t="shared" si="7"/>
@@ -35155,7 +35186,7 @@
         <v>35</v>
       </c>
       <c r="F141" s="97" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G141" s="98">
         <v>1</v>
@@ -35222,7 +35253,7 @@
         <v>2</v>
       </c>
       <c r="C142" s="118" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D142" s="97" t="str">
         <f t="shared" si="7"/>
@@ -35267,7 +35298,7 @@
         <v>3</v>
       </c>
       <c r="C143" s="118" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D143" s="97" t="str">
         <f t="shared" si="7"/>
@@ -35300,12 +35331,12 @@
         <v>86</v>
       </c>
       <c r="S143" s="119" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="T143" s="109"/>
       <c r="U143" s="109"/>
       <c r="V143" s="109" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="W143" s="100" t="s">
         <v>43</v>
@@ -35352,7 +35383,7 @@
         <v>3</v>
       </c>
       <c r="C144" s="118" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D144" s="97" t="str">
         <f t="shared" si="7"/>
@@ -35429,7 +35460,7 @@
         <v>3</v>
       </c>
       <c r="C145" s="118" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D145" s="97" t="str">
         <f t="shared" si="7"/>
@@ -35459,7 +35490,7 @@
       <c r="T145" s="109"/>
       <c r="U145" s="109"/>
       <c r="V145" s="109" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="W145" s="100" t="s">
         <v>43</v>
@@ -35508,7 +35539,7 @@
         <v>3</v>
       </c>
       <c r="C146" s="118" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D146" s="97" t="str">
         <f t="shared" si="7"/>
@@ -35585,7 +35616,7 @@
         <v>3</v>
       </c>
       <c r="C147" s="118" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D147" s="97" t="str">
         <f t="shared" si="7"/>
@@ -35662,7 +35693,7 @@
         <v>2</v>
       </c>
       <c r="C148" s="118" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D148" s="97" t="str">
         <f t="shared" si="7"/>
@@ -35707,7 +35738,7 @@
         <v>3</v>
       </c>
       <c r="C149" s="118" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D149" s="97" t="str">
         <f t="shared" si="7"/>
@@ -35784,7 +35815,7 @@
         <v>3</v>
       </c>
       <c r="C150" s="118" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D150" s="97" t="str">
         <f t="shared" si="7"/>
@@ -35808,7 +35839,7 @@
       </c>
       <c r="L150" s="109"/>
       <c r="M150" s="119" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="N150" s="109">
         <v>3417</v>
@@ -35831,7 +35862,7 @@
       <c r="T150" s="109"/>
       <c r="U150" s="109"/>
       <c r="V150" s="109" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="W150" s="100" t="s">
         <v>43</v>
@@ -35880,7 +35911,7 @@
         <v>3</v>
       </c>
       <c r="C151" s="118" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D151" s="97" t="str">
         <f t="shared" si="7"/>
@@ -35925,7 +35956,7 @@
         <v>4</v>
       </c>
       <c r="C152" s="118" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D152" s="97" t="str">
         <f t="shared" si="7"/>
@@ -35951,7 +35982,7 @@
         <v>98</v>
       </c>
       <c r="M152" s="119" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="N152" s="109">
         <v>3417</v>
@@ -36028,7 +36059,7 @@
         <v>4</v>
       </c>
       <c r="C153" s="118" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D153" s="97" t="str">
         <f t="shared" si="7"/>
@@ -36054,7 +36085,7 @@
         <v>98</v>
       </c>
       <c r="M153" s="119" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="N153" s="109">
         <v>3417</v>
@@ -36124,7 +36155,7 @@
         <v>4</v>
       </c>
       <c r="C154" s="118" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D154" s="97" t="str">
         <f t="shared" si="7"/>
@@ -36150,7 +36181,7 @@
         <v>98</v>
       </c>
       <c r="M154" s="119" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="N154" s="109">
         <v>3417</v>
@@ -36220,7 +36251,7 @@
         <v>3</v>
       </c>
       <c r="C155" s="118" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="D155" s="97" t="str">
         <f t="shared" si="7"/>
@@ -36246,7 +36277,7 @@
         <v>80</v>
       </c>
       <c r="M155" s="119" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="N155" s="109">
         <v>201049.28</v>
@@ -36265,13 +36296,13 @@
       </c>
       <c r="S155" s="119"/>
       <c r="T155" s="109" t="s">
+        <v>652</v>
+      </c>
+      <c r="U155" s="120" t="s">
         <v>653</v>
       </c>
-      <c r="U155" s="120" t="s">
+      <c r="V155" s="109" t="s">
         <v>654</v>
-      </c>
-      <c r="V155" s="109" t="s">
-        <v>655</v>
       </c>
       <c r="W155" s="100" t="s">
         <v>43</v>
@@ -36320,7 +36351,7 @@
         <v>2</v>
       </c>
       <c r="C156" s="118" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D156" s="97" t="str">
         <f t="shared" si="7"/>
@@ -36365,7 +36396,7 @@
         <v>3</v>
       </c>
       <c r="C157" s="118" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D157" s="97" t="str">
         <f t="shared" si="7"/>
@@ -36442,7 +36473,7 @@
         <v>3</v>
       </c>
       <c r="C158" s="118" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D158" s="97" t="str">
         <f t="shared" si="7"/>
@@ -36519,7 +36550,7 @@
         <v>3</v>
       </c>
       <c r="C159" s="118" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D159" s="97" t="str">
         <f t="shared" si="7"/>
@@ -36596,7 +36627,7 @@
         <v>2</v>
       </c>
       <c r="C160" s="118" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D160" s="97" t="str">
         <f t="shared" si="7"/>
@@ -36641,7 +36672,7 @@
         <v>3</v>
       </c>
       <c r="C161" s="118" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D161" s="97" t="str">
         <f t="shared" si="7"/>
@@ -36651,7 +36682,7 @@
         <v>35</v>
       </c>
       <c r="F161" s="97" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G161" s="98">
         <v>1</v>
@@ -36718,7 +36749,7 @@
         <v>3</v>
       </c>
       <c r="C162" s="118" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D162" s="97" t="str">
         <f t="shared" si="7"/>
@@ -36728,7 +36759,7 @@
         <v>35</v>
       </c>
       <c r="F162" s="97" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G162" s="98">
         <v>0.1</v>
@@ -36795,7 +36826,7 @@
         <v>3</v>
       </c>
       <c r="C163" s="118" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D163" s="97" t="str">
         <f t="shared" si="7"/>
@@ -36805,7 +36836,7 @@
         <v>35</v>
       </c>
       <c r="F163" s="97" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G163" s="98">
         <v>0.1</v>
@@ -36872,7 +36903,7 @@
         <v>2</v>
       </c>
       <c r="C164" s="118" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D164" s="97" t="str">
         <f t="shared" si="7"/>
@@ -36917,7 +36948,7 @@
         <v>3</v>
       </c>
       <c r="C165" s="118" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D165" s="97" t="str">
         <f t="shared" si="7"/>
@@ -36994,7 +37025,7 @@
         <v>3</v>
       </c>
       <c r="C166" s="118" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D166" s="97" t="str">
         <f t="shared" si="7"/>
@@ -37071,7 +37102,7 @@
         <v>3</v>
       </c>
       <c r="C167" s="118" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D167" s="97" t="str">
         <f t="shared" si="7"/>
@@ -37148,7 +37179,7 @@
         <v>3</v>
       </c>
       <c r="C168" s="118" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="D168" s="97" t="str">
         <f t="shared" si="7"/>
@@ -37225,7 +37256,7 @@
         <v>3</v>
       </c>
       <c r="C169" s="118" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D169" s="97" t="str">
         <f t="shared" si="7"/>
@@ -37302,7 +37333,7 @@
         <v>3</v>
       </c>
       <c r="C170" s="118" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="D170" s="97" t="str">
         <f t="shared" si="7"/>
@@ -37379,7 +37410,7 @@
         <v>1</v>
       </c>
       <c r="C171" s="118" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="D171" s="97" t="str">
         <f t="shared" si="7"/>
@@ -37424,7 +37455,7 @@
         <v>2</v>
       </c>
       <c r="C172" s="118" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="D172" s="97" t="str">
         <f t="shared" si="7"/>
@@ -37469,7 +37500,7 @@
         <v>3</v>
       </c>
       <c r="C173" s="118" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D173" s="97" t="str">
         <f t="shared" si="7"/>
@@ -37544,7 +37575,7 @@
         <v>3</v>
       </c>
       <c r="C174" s="118" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="D174" s="97" t="str">
         <f t="shared" si="7"/>
@@ -37577,12 +37608,12 @@
         <v>86</v>
       </c>
       <c r="S174" s="119" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="T174" s="109"/>
       <c r="U174" s="109"/>
       <c r="V174" s="109" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="W174" s="100" t="s">
         <v>43</v>
@@ -37629,7 +37660,7 @@
         <v>3</v>
       </c>
       <c r="C175" s="118" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D175" s="97" t="str">
         <f t="shared" si="7"/>
@@ -37662,12 +37693,12 @@
         <v>86</v>
       </c>
       <c r="S175" s="119" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="T175" s="109"/>
       <c r="U175" s="109"/>
       <c r="V175" s="109" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="W175" s="100" t="s">
         <v>43</v>
@@ -37714,7 +37745,7 @@
         <v>3</v>
       </c>
       <c r="C176" s="118" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D176" s="97" t="str">
         <f t="shared" si="7"/>
@@ -37747,12 +37778,12 @@
         <v>86</v>
       </c>
       <c r="S176" s="119" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="T176" s="109"/>
       <c r="U176" s="109"/>
       <c r="V176" s="109" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="W176" s="100" t="s">
         <v>43</v>
@@ -37799,7 +37830,7 @@
         <v>3</v>
       </c>
       <c r="C177" s="118" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D177" s="97" t="str">
         <f t="shared" si="7"/>
@@ -37876,7 +37907,7 @@
         <v>3</v>
       </c>
       <c r="C178" s="118" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D178" s="97" t="str">
         <f t="shared" si="7"/>
@@ -37953,7 +37984,7 @@
         <v>2</v>
       </c>
       <c r="C179" s="118" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="D179" s="97" t="str">
         <f t="shared" si="7"/>
@@ -37998,7 +38029,7 @@
         <v>3</v>
       </c>
       <c r="C180" s="118" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D180" s="97" t="str">
         <f t="shared" ref="D180:D243" si="14">REPT("   ", B180*2) &amp; C180</f>
@@ -38008,7 +38039,7 @@
         <v>35</v>
       </c>
       <c r="F180" s="97" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G180" s="98">
         <v>6</v>
@@ -38031,12 +38062,12 @@
         <v>86</v>
       </c>
       <c r="S180" s="119" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="T180" s="109"/>
       <c r="U180" s="109"/>
       <c r="V180" s="109" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="W180" s="100" t="s">
         <v>43</v>
@@ -38083,7 +38114,7 @@
         <v>3</v>
       </c>
       <c r="C181" s="118" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D181" s="97" t="str">
         <f t="shared" si="14"/>
@@ -38093,7 +38124,7 @@
         <v>35</v>
       </c>
       <c r="F181" s="97" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G181" s="98">
         <v>1</v>
@@ -38160,7 +38191,7 @@
         <v>3</v>
       </c>
       <c r="C182" s="118" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D182" s="97" t="str">
         <f t="shared" si="14"/>
@@ -38170,7 +38201,7 @@
         <v>35</v>
       </c>
       <c r="F182" s="97" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G182" s="98">
         <v>1</v>
@@ -38190,7 +38221,7 @@
       <c r="T182" s="109"/>
       <c r="U182" s="109"/>
       <c r="V182" s="109" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="W182" s="100" t="s">
         <v>43</v>
@@ -38239,7 +38270,7 @@
         <v>3</v>
       </c>
       <c r="C183" s="118" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D183" s="97" t="str">
         <f t="shared" si="14"/>
@@ -38249,7 +38280,7 @@
         <v>35</v>
       </c>
       <c r="F183" s="97" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G183" s="98">
         <v>1</v>
@@ -38316,7 +38347,7 @@
         <v>3</v>
       </c>
       <c r="C184" s="118" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D184" s="97" t="str">
         <f t="shared" si="14"/>
@@ -38326,7 +38357,7 @@
         <v>35</v>
       </c>
       <c r="F184" s="97" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G184" s="98">
         <v>1</v>
@@ -38400,7 +38431,7 @@
         <v>2</v>
       </c>
       <c r="C185" s="118" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="D185" s="97" t="str">
         <f t="shared" si="14"/>
@@ -38452,7 +38483,7 @@
         <v>3</v>
       </c>
       <c r="C186" s="118" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D186" s="97" t="str">
         <f t="shared" si="14"/>
@@ -38536,7 +38567,7 @@
         <v>3</v>
       </c>
       <c r="C187" s="118" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="D187" s="97" t="str">
         <f t="shared" si="14"/>
@@ -38613,7 +38644,7 @@
         <v>3</v>
       </c>
       <c r="C188" s="118" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="D188" s="97" t="str">
         <f t="shared" si="14"/>
@@ -38690,7 +38721,7 @@
         <v>2</v>
       </c>
       <c r="C189" s="118" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D189" s="97" t="str">
         <f t="shared" si="14"/>
@@ -38735,7 +38766,7 @@
         <v>3</v>
       </c>
       <c r="C190" s="118" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D190" s="97" t="str">
         <f t="shared" si="14"/>
@@ -38812,7 +38843,7 @@
         <v>3</v>
       </c>
       <c r="C191" s="118" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D191" s="97" t="str">
         <f t="shared" si="14"/>
@@ -38836,7 +38867,7 @@
       </c>
       <c r="L191" s="109"/>
       <c r="M191" s="119" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="N191" s="109">
         <v>3417</v>
@@ -38859,7 +38890,7 @@
       <c r="T191" s="109"/>
       <c r="U191" s="109"/>
       <c r="V191" s="109" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="W191" s="100" t="s">
         <v>43</v>
@@ -38908,7 +38939,7 @@
         <v>3</v>
       </c>
       <c r="C192" s="118" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D192" s="97" t="str">
         <f t="shared" si="14"/>
@@ -38953,7 +38984,7 @@
         <v>4</v>
       </c>
       <c r="C193" s="118" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D193" s="97" t="str">
         <f t="shared" si="14"/>
@@ -38979,7 +39010,7 @@
         <v>98</v>
       </c>
       <c r="M193" s="119" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="N193" s="109">
         <v>3417</v>
@@ -39049,7 +39080,7 @@
         <v>4</v>
       </c>
       <c r="C194" s="118" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D194" s="97" t="str">
         <f t="shared" si="14"/>
@@ -39075,7 +39106,7 @@
         <v>98</v>
       </c>
       <c r="M194" s="119" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="N194" s="109">
         <v>3417</v>
@@ -39145,7 +39176,7 @@
         <v>4</v>
       </c>
       <c r="C195" s="118" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D195" s="97" t="str">
         <f t="shared" si="14"/>
@@ -39171,7 +39202,7 @@
         <v>98</v>
       </c>
       <c r="M195" s="119" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="N195" s="109">
         <v>3417</v>
@@ -39241,7 +39272,7 @@
         <v>3</v>
       </c>
       <c r="C196" s="118" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="D196" s="97" t="str">
         <f t="shared" si="14"/>
@@ -39267,7 +39298,7 @@
         <v>80</v>
       </c>
       <c r="M196" s="119" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="N196" s="109">
         <v>201049.28</v>
@@ -39286,13 +39317,13 @@
       </c>
       <c r="S196" s="119"/>
       <c r="T196" s="109" t="s">
+        <v>652</v>
+      </c>
+      <c r="U196" s="120" t="s">
         <v>653</v>
       </c>
-      <c r="U196" s="120" t="s">
+      <c r="V196" s="109" t="s">
         <v>654</v>
-      </c>
-      <c r="V196" s="109" t="s">
-        <v>655</v>
       </c>
       <c r="W196" s="100" t="s">
         <v>43</v>
@@ -39341,7 +39372,7 @@
         <v>2</v>
       </c>
       <c r="C197" s="118" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D197" s="97" t="str">
         <f t="shared" si="14"/>
@@ -39386,7 +39417,7 @@
         <v>3</v>
       </c>
       <c r="C198" s="118" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D198" s="97" t="str">
         <f t="shared" si="14"/>
@@ -39463,7 +39494,7 @@
         <v>3</v>
       </c>
       <c r="C199" s="118" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D199" s="97" t="str">
         <f t="shared" si="14"/>
@@ -39540,7 +39571,7 @@
         <v>3</v>
       </c>
       <c r="C200" s="118" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D200" s="97" t="str">
         <f t="shared" si="14"/>
@@ -39617,7 +39648,7 @@
         <v>3</v>
       </c>
       <c r="C201" s="118" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="D201" s="97" t="str">
         <f t="shared" si="14"/>
@@ -39694,7 +39725,7 @@
         <v>3</v>
       </c>
       <c r="C202" s="118" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D202" s="97" t="str">
         <f t="shared" si="14"/>
@@ -39771,7 +39802,7 @@
         <v>3</v>
       </c>
       <c r="C203" s="118" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="D203" s="97" t="str">
         <f t="shared" si="14"/>
@@ -39848,7 +39879,7 @@
         <v>1</v>
       </c>
       <c r="C204" s="118" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="D204" s="97" t="str">
         <f t="shared" si="14"/>
@@ -39893,7 +39924,7 @@
         <v>2</v>
       </c>
       <c r="C205" s="118" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D205" s="97" t="str">
         <f t="shared" si="14"/>
@@ -39919,7 +39950,7 @@
         <v>98</v>
       </c>
       <c r="M205" s="119" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="N205" s="109">
         <v>3417</v>
@@ -39989,7 +40020,7 @@
         <v>2</v>
       </c>
       <c r="C206" s="118" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D206" s="97" t="str">
         <f t="shared" si="14"/>
@@ -40015,7 +40046,7 @@
         <v>98</v>
       </c>
       <c r="M206" s="119" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="N206" s="109">
         <v>3417</v>
@@ -40085,7 +40116,7 @@
         <v>2</v>
       </c>
       <c r="C207" s="118" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D207" s="97" t="str">
         <f t="shared" si="14"/>
@@ -40111,7 +40142,7 @@
         <v>98</v>
       </c>
       <c r="M207" s="119" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="N207" s="109">
         <v>3417</v>
@@ -40188,7 +40219,7 @@
         <v>2</v>
       </c>
       <c r="C208" s="118" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D208" s="97" t="str">
         <f t="shared" si="14"/>
@@ -40240,7 +40271,7 @@
         <v>3</v>
       </c>
       <c r="C209" s="118" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D209" s="97" t="str">
         <f t="shared" si="14"/>
@@ -40324,7 +40355,7 @@
         <v>3</v>
       </c>
       <c r="C210" s="118" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D210" s="97" t="str">
         <f t="shared" si="14"/>
@@ -40348,7 +40379,7 @@
       </c>
       <c r="L210" s="109"/>
       <c r="M210" s="119" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="N210" s="109">
         <v>3417</v>
@@ -40371,7 +40402,7 @@
       <c r="T210" s="109"/>
       <c r="U210" s="109"/>
       <c r="V210" s="109" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="W210" s="100" t="s">
         <v>43</v>
@@ -40420,7 +40451,7 @@
         <v>3</v>
       </c>
       <c r="C211" s="118" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="D211" s="97" t="str">
         <f t="shared" si="14"/>
@@ -40446,7 +40477,7 @@
         <v>80</v>
       </c>
       <c r="M211" s="119" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="N211" s="109">
         <v>201049.28</v>
@@ -40465,13 +40496,13 @@
       </c>
       <c r="S211" s="119"/>
       <c r="T211" s="109" t="s">
+        <v>652</v>
+      </c>
+      <c r="U211" s="120" t="s">
         <v>653</v>
       </c>
-      <c r="U211" s="120" t="s">
+      <c r="V211" s="109" t="s">
         <v>654</v>
-      </c>
-      <c r="V211" s="109" t="s">
-        <v>655</v>
       </c>
       <c r="W211" s="100" t="s">
         <v>43</v>
@@ -40520,7 +40551,7 @@
         <v>3</v>
       </c>
       <c r="C212" s="118" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D212" s="97" t="str">
         <f t="shared" si="14"/>
@@ -40597,7 +40628,7 @@
         <v>2</v>
       </c>
       <c r="C213" s="118" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D213" s="97" t="str">
         <f t="shared" si="14"/>
@@ -40642,7 +40673,7 @@
         <v>3</v>
       </c>
       <c r="C214" s="118" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D214" s="97" t="str">
         <f t="shared" si="14"/>
@@ -40652,7 +40683,7 @@
         <v>35</v>
       </c>
       <c r="F214" s="97" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G214" s="98">
         <v>1</v>
@@ -40719,7 +40750,7 @@
         <v>3</v>
       </c>
       <c r="C215" s="118" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D215" s="97" t="str">
         <f t="shared" si="14"/>
@@ -40729,7 +40760,7 @@
         <v>35</v>
       </c>
       <c r="F215" s="97" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G215" s="98">
         <v>0.1</v>
@@ -40796,7 +40827,7 @@
         <v>3</v>
       </c>
       <c r="C216" s="118" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D216" s="97" t="str">
         <f t="shared" si="14"/>
@@ -40806,7 +40837,7 @@
         <v>35</v>
       </c>
       <c r="F216" s="97" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G216" s="98">
         <v>0.1</v>
@@ -40873,7 +40904,7 @@
         <v>2</v>
       </c>
       <c r="C217" s="118" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D217" s="97" t="str">
         <f t="shared" si="14"/>
@@ -40918,7 +40949,7 @@
         <v>3</v>
       </c>
       <c r="C218" s="118" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D218" s="97" t="str">
         <f t="shared" si="14"/>
@@ -40995,7 +41026,7 @@
         <v>3</v>
       </c>
       <c r="C219" s="118" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D219" s="97" t="str">
         <f t="shared" si="14"/>
@@ -41072,7 +41103,7 @@
         <v>3</v>
       </c>
       <c r="C220" s="118" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D220" s="97" t="str">
         <f t="shared" si="14"/>
@@ -41149,7 +41180,7 @@
         <v>3</v>
       </c>
       <c r="C221" s="118" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="D221" s="97" t="str">
         <f t="shared" si="14"/>
@@ -41226,7 +41257,7 @@
         <v>3</v>
       </c>
       <c r="C222" s="118" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D222" s="97" t="str">
         <f t="shared" si="14"/>
@@ -41303,7 +41334,7 @@
         <v>3</v>
       </c>
       <c r="C223" s="118" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="D223" s="97" t="str">
         <f t="shared" si="14"/>
@@ -41451,7 +41482,7 @@
         <v>50</v>
       </c>
       <c r="M225" s="104" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="N225" s="109">
         <v>1144</v>
@@ -41537,7 +41568,7 @@
         <v>50</v>
       </c>
       <c r="M226" s="104" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="N226" s="109">
         <v>1144</v>
@@ -41626,7 +41657,7 @@
         <v>50</v>
       </c>
       <c r="M227" s="104" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="N227" s="109">
         <v>1144</v>
@@ -41715,7 +41746,7 @@
         <v>50</v>
       </c>
       <c r="M228" s="104" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="N228" s="109">
         <v>1144</v>
@@ -41797,7 +41828,7 @@
         <v>50</v>
       </c>
       <c r="M229" s="104" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="N229" s="109">
         <v>1144</v>
@@ -41879,7 +41910,7 @@
         <v>50</v>
       </c>
       <c r="M230" s="104" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="N230" s="109">
         <v>1144</v>
@@ -41935,7 +41966,7 @@
         <v>1</v>
       </c>
       <c r="C231" s="119" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="D231" s="97" t="str">
         <f t="shared" si="14"/>
@@ -41980,7 +42011,7 @@
         <v>2</v>
       </c>
       <c r="C232" s="119" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="D232" s="97" t="str">
         <f t="shared" si="14"/>
@@ -42057,7 +42088,7 @@
         <v>1</v>
       </c>
       <c r="C233" s="119" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="D233" s="97" t="str">
         <f t="shared" si="14"/>
@@ -42102,7 +42133,7 @@
         <v>2</v>
       </c>
       <c r="C234" s="119" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D234" s="97" t="str">
         <f t="shared" si="14"/>
@@ -42147,7 +42178,7 @@
         <v>3</v>
       </c>
       <c r="C235" s="119" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D235" s="97" t="str">
         <f t="shared" si="14"/>
@@ -42157,7 +42188,7 @@
         <v>35</v>
       </c>
       <c r="F235" s="97" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="G235" s="98">
         <v>1</v>
@@ -42224,7 +42255,7 @@
         <v>2</v>
       </c>
       <c r="C236" s="119" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D236" s="97" t="str">
         <f t="shared" si="14"/>
@@ -42269,7 +42300,7 @@
         <v>3</v>
       </c>
       <c r="C237" s="119" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="D237" s="97" t="str">
         <f t="shared" si="14"/>
@@ -42279,7 +42310,7 @@
         <v>35</v>
       </c>
       <c r="F237" s="97" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="G237" s="98">
         <v>1</v>
@@ -42346,7 +42377,7 @@
         <v>3</v>
       </c>
       <c r="C238" s="119" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D238" s="97" t="str">
         <f t="shared" si="14"/>
@@ -42356,7 +42387,7 @@
         <v>35</v>
       </c>
       <c r="F238" s="97" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="G238" s="98">
         <v>1</v>
@@ -42423,7 +42454,7 @@
         <v>3</v>
       </c>
       <c r="C239" s="119" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="D239" s="97" t="str">
         <f t="shared" si="14"/>
@@ -42433,7 +42464,7 @@
         <v>35</v>
       </c>
       <c r="F239" s="97" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="G239" s="98">
         <v>1</v>
@@ -42500,7 +42531,7 @@
         <v>2</v>
       </c>
       <c r="C240" s="119" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D240" s="97" t="str">
         <f t="shared" si="14"/>
@@ -43513,7 +43544,7 @@
         <v>2</v>
       </c>
       <c r="C257" s="118" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="D257" s="97" t="str">
         <f t="shared" si="32"/>
@@ -43560,7 +43591,7 @@
         <v>1</v>
       </c>
       <c r="C258" s="118" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D258" s="97" t="str">
         <f t="shared" si="32"/>
@@ -43605,7 +43636,7 @@
         <v>2</v>
       </c>
       <c r="C259" s="118" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D259" s="97" t="str">
         <f t="shared" si="32"/>
@@ -43650,7 +43681,7 @@
         <v>2</v>
       </c>
       <c r="C260" s="118" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D260" s="97" t="str">
         <f t="shared" si="32"/>
@@ -43695,7 +43726,7 @@
         <v>3</v>
       </c>
       <c r="C261" s="118" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D261" s="97" t="str">
         <f t="shared" si="32"/>
@@ -43770,7 +43801,7 @@
         <v>3</v>
       </c>
       <c r="C262" s="118" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D262" s="97" t="str">
         <f t="shared" si="32"/>
@@ -43815,7 +43846,7 @@
         <v>4</v>
       </c>
       <c r="C263" s="118" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D263" s="97" t="str">
         <f t="shared" si="32"/>
@@ -43825,7 +43856,7 @@
         <v>35</v>
       </c>
       <c r="F263" s="97" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="G263" s="98">
         <v>1</v>
@@ -43848,12 +43879,12 @@
         <v>153</v>
       </c>
       <c r="S263" s="119" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="T263" s="121"/>
       <c r="U263" s="120"/>
       <c r="V263" s="109" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="W263" s="100"/>
       <c r="X263" s="110">
@@ -43898,7 +43929,7 @@
         <v>4</v>
       </c>
       <c r="C264" s="118" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D264" s="97" t="str">
         <f t="shared" si="32"/>
@@ -43908,7 +43939,7 @@
         <v>35</v>
       </c>
       <c r="F264" s="97" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="G264" s="98">
         <v>1</v>
@@ -43931,7 +43962,7 @@
         <v>153</v>
       </c>
       <c r="S264" s="119" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="T264" s="121"/>
       <c r="U264" s="120"/>
@@ -43979,7 +44010,7 @@
         <v>4</v>
       </c>
       <c r="C265" s="118" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D265" s="97" t="str">
         <f t="shared" si="32"/>
@@ -43989,7 +44020,7 @@
         <v>35</v>
       </c>
       <c r="F265" s="97" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="G265" s="98">
         <v>1</v>
@@ -44012,12 +44043,12 @@
         <v>153</v>
       </c>
       <c r="S265" s="119" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="T265" s="121"/>
       <c r="U265" s="120"/>
       <c r="V265" s="109" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="W265" s="100"/>
       <c r="X265" s="110">
@@ -44062,7 +44093,7 @@
         <v>3</v>
       </c>
       <c r="C266" s="118" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D266" s="97" t="str">
         <f t="shared" si="32"/>
@@ -44251,6 +44282,8 @@
     <mergeCell ref="U112:U114"/>
     <mergeCell ref="T122:T124"/>
     <mergeCell ref="S67:S69"/>
+    <mergeCell ref="T67:T69"/>
+    <mergeCell ref="T127:T129"/>
     <mergeCell ref="S18:S20"/>
     <mergeCell ref="U122:U124"/>
     <mergeCell ref="U18:U20"/>
@@ -44267,7 +44300,6 @@
     <mergeCell ref="T28:T30"/>
     <mergeCell ref="S45:S47"/>
     <mergeCell ref="S79:S81"/>
-    <mergeCell ref="T67:T69"/>
     <mergeCell ref="U3:U4"/>
     <mergeCell ref="T57:T59"/>
     <mergeCell ref="T33:T35"/>
@@ -44294,7 +44326,6 @@
     <mergeCell ref="S52:S54"/>
     <mergeCell ref="S86:S88"/>
     <mergeCell ref="U86:U88"/>
-    <mergeCell ref="T127:T129"/>
     <mergeCell ref="S23:S25"/>
     <mergeCell ref="S225:S230"/>
     <mergeCell ref="S122:S124"/>

</xml_diff>